<commit_message>
16 enero 2022 II
</commit_message>
<xml_diff>
--- a/ocultos/menu.xlsx
+++ b/ocultos/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\pp\Kaizen\ocultos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A34010F-31C1-49BE-806C-5387B0D75A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D843958-DA67-4286-BC2F-FAF91CCEC811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8E7E0398-F09C-401C-9437-51E251C0AA9A}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -578,6 +579,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -590,8 +593,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1047,7 +1048,7 @@
   <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K4" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,20 +1069,20 @@
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -1127,7 +1128,7 @@
       <c r="P6" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" s="16" t="s">
+      <c r="Q6" s="18" t="s">
         <v>14</v>
       </c>
       <c r="R6" t="s">
@@ -1157,7 +1158,7 @@
       <c r="I7" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="14" t="s">
         <v>17</v>
       </c>
       <c r="L7" s="3" t="s">
@@ -1175,7 +1176,7 @@
       <c r="P7" t="s">
         <v>22</v>
       </c>
-      <c r="Q7" s="17"/>
+      <c r="Q7" s="19"/>
       <c r="R7" t="s">
         <v>23</v>
       </c>
@@ -1188,7 +1189,7 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="14" t="s">
         <v>25</v>
       </c>
       <c r="L8" t="s">
@@ -1206,7 +1207,7 @@
       <c r="P8" t="s">
         <v>30</v>
       </c>
-      <c r="Q8" s="17"/>
+      <c r="Q8" s="19"/>
       <c r="R8" t="s">
         <v>31</v>
       </c>
@@ -1219,7 +1220,7 @@
       <c r="E9" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="15" t="s">
         <v>34</v>
       </c>
       <c r="L9" s="4" t="s">
@@ -1237,7 +1238,7 @@
       <c r="P9" t="s">
         <v>38</v>
       </c>
-      <c r="Q9" s="17"/>
+      <c r="Q9" s="19"/>
       <c r="R9" t="s">
         <v>39</v>
       </c>
@@ -1250,7 +1251,7 @@
       <c r="E10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="K10" s="14" t="s">
         <v>42</v>
       </c>
       <c r="L10" t="s">
@@ -1268,7 +1269,7 @@
       <c r="P10" t="s">
         <v>47</v>
       </c>
-      <c r="Q10" s="17"/>
+      <c r="Q10" s="19"/>
       <c r="R10" t="s">
         <v>48</v>
       </c>
@@ -1281,7 +1282,7 @@
       <c r="E11" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="14" t="s">
         <v>51</v>
       </c>
       <c r="L11" t="s">
@@ -1296,7 +1297,7 @@
       <c r="P11" t="s">
         <v>54</v>
       </c>
-      <c r="Q11" s="17"/>
+      <c r="Q11" s="19"/>
       <c r="R11" t="s">
         <v>55</v>
       </c>
@@ -1306,7 +1307,7 @@
       <c r="D12" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="14" t="s">
         <v>57</v>
       </c>
       <c r="L12" t="s">
@@ -1318,13 +1319,13 @@
       <c r="P12" t="s">
         <v>60</v>
       </c>
-      <c r="Q12" s="17"/>
+      <c r="Q12" s="19"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="K13" s="14" t="s">
         <v>61</v>
       </c>
       <c r="L13" t="s">
@@ -1339,13 +1340,13 @@
       <c r="P13" t="s">
         <v>65</v>
       </c>
-      <c r="Q13" s="17"/>
+      <c r="Q13" s="19"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>66</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="14" t="s">
         <v>67</v>
       </c>
       <c r="L14" t="s">
@@ -1357,13 +1358,13 @@
       <c r="P14" t="s">
         <v>70</v>
       </c>
-      <c r="Q14" s="17"/>
+      <c r="Q14" s="19"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>71</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="14" t="s">
         <v>72</v>
       </c>
       <c r="L15" s="11" t="s">
@@ -1377,7 +1378,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K16" t="s">
+      <c r="K16" s="14" t="s">
         <v>75</v>
       </c>
       <c r="L16" s="12" t="s">
@@ -1388,7 +1389,7 @@
       </c>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="K17" t="s">
+      <c r="K17" s="14" t="s">
         <v>77</v>
       </c>
       <c r="L17" s="12" t="s">
@@ -1405,7 +1406,7 @@
       <c r="D18" t="s">
         <v>80</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="14" t="s">
         <v>81</v>
       </c>
       <c r="L18" s="12" t="s">
@@ -1419,7 +1420,7 @@
       </c>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="K19" t="s">
+      <c r="K19" s="14" t="s">
         <v>85</v>
       </c>
       <c r="L19" s="12" t="s">
@@ -1529,11 +1530,11 @@
       </c>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
       <c r="M30" s="9" t="s">
         <v>50</v>
       </c>
@@ -1551,11 +1552,11 @@
       </c>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
       <c r="K32" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
16 enero 2022 III
</commit_message>
<xml_diff>
--- a/ocultos/menu.xlsx
+++ b/ocultos/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\pp\Kaizen\ocultos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D843958-DA67-4286-BC2F-FAF91CCEC811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF424C6-08EB-49AB-A300-F9172CC4A556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8E7E0398-F09C-401C-9437-51E251C0AA9A}"/>
   </bookViews>
@@ -1047,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D2A24A-8103-4448-8D8A-5190A8AC0349}">
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K4" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="K16" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,7 +1450,7 @@
       </c>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="K22" t="s">
+      <c r="K22" s="14" t="s">
         <v>92</v>
       </c>
       <c r="L22" s="12" t="s">
@@ -1461,7 +1461,7 @@
       </c>
     </row>
     <row r="23" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="K23" t="s">
+      <c r="K23" s="14" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1472,7 +1472,7 @@
       <c r="D24" t="s">
         <v>97</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="14" t="s">
         <v>98</v>
       </c>
       <c r="L24" t="s">
@@ -1484,7 +1484,7 @@
       <c r="N24" s="10"/>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="K25" t="s">
+      <c r="K25" s="14" t="s">
         <v>100</v>
       </c>
       <c r="L25" t="s">
@@ -1495,7 +1495,7 @@
       </c>
     </row>
     <row r="26" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="K26" t="s">
+      <c r="K26" s="14" t="s">
         <v>103</v>
       </c>
       <c r="L26" t="s">
@@ -1506,7 +1506,7 @@
       </c>
     </row>
     <row r="27" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="K27" t="s">
+      <c r="K27" s="14" t="s">
         <v>106</v>
       </c>
       <c r="L27" t="s">
@@ -1517,7 +1517,7 @@
       </c>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="K28" t="s">
+      <c r="K28" s="14" t="s">
         <v>109</v>
       </c>
       <c r="L28" t="s">
@@ -1525,7 +1525,7 @@
       </c>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="K29" t="s">
+      <c r="K29" s="14" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
16 enero 2022 IV
</commit_message>
<xml_diff>
--- a/ocultos/menu.xlsx
+++ b/ocultos/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\pp\Kaizen\ocultos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF424C6-08EB-49AB-A300-F9172CC4A556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9E91D6-1F5D-4997-BBD6-958443CCF282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8E7E0398-F09C-401C-9437-51E251C0AA9A}"/>
   </bookViews>
@@ -1047,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D2A24A-8103-4448-8D8A-5190A8AC0349}">
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K16" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" topLeftCell="K19" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,7 +1544,7 @@
       <c r="C31" t="s">
         <v>113</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="14" t="s">
         <v>114</v>
       </c>
       <c r="M31" t="s">
@@ -1557,7 +1557,7 @@
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
-      <c r="K32" t="s">
+      <c r="K32" s="14" t="s">
         <v>117</v>
       </c>
       <c r="M32" t="s">

</xml_diff>